<commit_message>
update algorithm of nav
</commit_message>
<xml_diff>
--- a/result/rp/evaluation.xlsx
+++ b/result/rp/evaluation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>RP</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>20100105-20141205</t>
+  </si>
+  <si>
+    <t>20150106-20180523</t>
+  </si>
+  <si>
+    <t>20150106-20210805</t>
   </si>
   <si>
     <t>20110906-20150731</t>
@@ -482,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,7 +528,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>3.577855772692229</v>
+        <v>3.568928571180563</v>
       </c>
       <c r="C2">
         <v>-0.8006820438348328</v>
@@ -551,7 +557,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>2.869004667648634</v>
+        <v>2.861963093059283</v>
       </c>
       <c r="C3">
         <v>1.304727661782357</v>
@@ -583,7 +589,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>5.760942288930138</v>
+        <v>5.755777680552265</v>
       </c>
       <c r="C4">
         <v>3.882433787815698</v>
@@ -615,7 +621,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>-0.2174841080655576</v>
+        <v>-0.2246310595382273</v>
       </c>
       <c r="C5">
         <v>-3.397059047952677</v>
@@ -647,7 +653,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>14.45343646243047</v>
+        <v>14.44778433313772</v>
       </c>
       <c r="C6">
         <v>17.75905335550287</v>
@@ -679,7 +685,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>10.74263728990026</v>
+        <v>10.73528321106567</v>
       </c>
       <c r="C7">
         <v>8.269709494039379</v>
@@ -711,7 +717,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>2.472908854891132</v>
+        <v>2.466727039294203</v>
       </c>
       <c r="C8">
         <v>0.08444352419667567</v>
@@ -743,7 +749,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>3.240643885338956</v>
+        <v>3.233788816510241</v>
       </c>
       <c r="C9">
         <v>2.615083958955733</v>
@@ -775,7 +781,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>5.546533979708324</v>
+        <v>5.53894955814358</v>
       </c>
       <c r="C10">
         <v>2.3296419480624</v>
@@ -807,7 +813,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>7.784788871987258</v>
+        <v>7.777982817134999</v>
       </c>
       <c r="C11">
         <v>9.656605743058844</v>
@@ -839,7 +845,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>5.760876590962294</v>
+        <v>5.755510281728782</v>
       </c>
       <c r="C12">
         <v>8.214778929470068</v>
@@ -871,7 +877,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>4.155242362194844</v>
+        <v>4.149900657287953</v>
       </c>
       <c r="C13">
         <v>3.747690858206165</v>
@@ -899,392 +905,387 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="1">
-        <v>2022</v>
+      <c r="A14" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>84.94018208822101</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>63.8308575101282</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>61.73903545008017</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>59.64721339003214</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>78.71809889625926</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>80.56543399051242</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>79.94064437435442</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>282.0370353245317</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>50.62118168026571</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>85.07479963695263</v>
+        <v>5.455410414492023</v>
       </c>
       <c r="C15">
-        <v>63.8308575101282</v>
+        <v>4.357020751422613</v>
       </c>
       <c r="D15">
-        <v>61.73903545008017</v>
+        <v>4.241233374730768</v>
       </c>
       <c r="E15">
-        <v>59.64721339003214</v>
+        <v>4.124069682630971</v>
       </c>
       <c r="F15">
-        <v>78.71809889625926</v>
+        <v>5.144091254013694</v>
       </c>
       <c r="G15">
-        <v>80.56543399051242</v>
+        <v>5.237542285940622</v>
       </c>
       <c r="H15">
-        <v>79.94064437435442</v>
+        <v>5.206034242990731</v>
+      </c>
+      <c r="I15">
+        <v>12.7339835969142</v>
       </c>
       <c r="J15">
-        <v>50.62118168026571</v>
+        <v>3.601870960674192</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>5.106141981918699</v>
+        <v>2.095943762271863</v>
       </c>
       <c r="C16">
-        <v>4.074509223399891</v>
+        <v>4.339086163689695</v>
       </c>
       <c r="D16">
-        <v>3.966371402856073</v>
+        <v>2.704544491311172</v>
       </c>
       <c r="E16">
-        <v>3.856940421995847</v>
+        <v>2.130711748534584</v>
       </c>
       <c r="F16">
-        <v>4.809379832517857</v>
+        <v>1.029468659813999</v>
       </c>
       <c r="G16">
-        <v>4.896609756702697</v>
+        <v>22.72746547063657</v>
       </c>
       <c r="H16">
-        <v>4.867199779023812</v>
+        <v>23.06289908286513</v>
+      </c>
+      <c r="I16">
+        <v>31.01924932297745</v>
       </c>
       <c r="J16">
-        <v>3.369111086363041</v>
+        <v>14.49362675912996</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>2.030023560514101</v>
+        <v>3.51525948187507</v>
       </c>
       <c r="C17">
-        <v>4.199362297935473</v>
+        <v>9.924291680870095</v>
       </c>
       <c r="D17">
-        <v>2.61791469153654</v>
+        <v>5.878770390395438</v>
       </c>
       <c r="E17">
-        <v>2.062784627011664</v>
+        <v>5.851804491363096</v>
       </c>
       <c r="F17">
-        <v>0.9991808602872699</v>
+        <v>2.939153560456676</v>
       </c>
       <c r="G17">
-        <v>21.99312905441591</v>
+        <v>46.0589391154498</v>
       </c>
       <c r="H17">
-        <v>22.31771854625275</v>
+        <v>43.7960007079443</v>
       </c>
       <c r="I17">
-        <v>29.98421243315283</v>
+        <v>69.22841798653275</v>
       </c>
       <c r="J17">
-        <v>14.02530445811948</v>
+        <v>44.8841110094541</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>3.511433553672966</v>
-      </c>
-      <c r="C18">
-        <v>9.924291680870095</v>
-      </c>
-      <c r="D18">
-        <v>5.878770390395438</v>
-      </c>
-      <c r="E18">
-        <v>5.851804491363096</v>
-      </c>
-      <c r="F18">
-        <v>2.939153560456676</v>
-      </c>
-      <c r="G18">
-        <v>46.0589391154498</v>
-      </c>
-      <c r="H18">
-        <v>43.7960007079443</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>44.8841110094541</v>
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" t="s">
-        <v>35</v>
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>377</v>
+      </c>
+      <c r="C19">
+        <v>945</v>
+      </c>
+      <c r="D19">
+        <v>540</v>
+      </c>
+      <c r="E19">
+        <v>615</v>
+      </c>
+      <c r="F19">
+        <v>424</v>
+      </c>
+      <c r="G19">
+        <v>1857</v>
+      </c>
+      <c r="H19">
+        <v>1795</v>
+      </c>
+      <c r="I19">
+        <v>2403</v>
+      </c>
+      <c r="J19">
+        <v>3174</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <v>377</v>
-      </c>
-      <c r="C20">
-        <v>945</v>
-      </c>
-      <c r="D20">
-        <v>540</v>
-      </c>
-      <c r="E20">
-        <v>615</v>
-      </c>
-      <c r="F20">
-        <v>424</v>
-      </c>
-      <c r="G20">
-        <v>1857</v>
-      </c>
-      <c r="H20">
-        <v>1795</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>3174</v>
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>1.887083889033322</v>
+      </c>
+      <c r="C21">
+        <v>0.6584231797497327</v>
+      </c>
+      <c r="D21">
+        <v>1.013528167393955</v>
+      </c>
+      <c r="E21">
+        <v>1.231488274098176</v>
+      </c>
+      <c r="F21">
+        <v>3.539434907305777</v>
+      </c>
+      <c r="G21">
+        <v>0.1644497423522739</v>
+      </c>
+      <c r="H21">
+        <v>0.1606917742863791</v>
+      </c>
+      <c r="I21">
+        <v>0.3621605172934003</v>
+      </c>
+      <c r="J21">
+        <v>0.1450193587615532</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>1.776316502137187</v>
+        <v>1.125179497256489</v>
       </c>
       <c r="C22">
-        <v>0.6130568727014324</v>
+        <v>0.2878786774336713</v>
       </c>
       <c r="D22">
-        <v>0.9420769909463469</v>
+        <v>0.4662857305391931</v>
       </c>
       <c r="E22">
-        <v>1.142545923864951</v>
+        <v>0.4484129374469236</v>
       </c>
       <c r="F22">
-        <v>3.311761451696861</v>
+        <v>1.239801595561394</v>
       </c>
       <c r="G22">
-        <v>0.1544388842720077</v>
+        <v>0.08114677070384042</v>
       </c>
       <c r="H22">
-        <v>0.1508749509745064</v>
+        <v>0.08462018725604226</v>
+      </c>
+      <c r="I22">
+        <v>0.162273928774549</v>
       </c>
       <c r="J22">
-        <v>0.1332661095046703</v>
+        <v>0.04682873806629837</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>1.02694219684923</v>
+        <v>29.65158951492512</v>
       </c>
       <c r="C23">
-        <v>0.2594122950993988</v>
+        <v>10.03385891922967</v>
       </c>
       <c r="D23">
-        <v>0.4195315152525712</v>
+        <v>15.85327071390837</v>
       </c>
       <c r="E23">
-        <v>0.402764676948246</v>
+        <v>19.85964832348571</v>
       </c>
       <c r="F23">
-        <v>1.125925261107338</v>
+        <v>50.64806829715589</v>
       </c>
       <c r="G23">
-        <v>0.07374469424316227</v>
+        <v>2.501991320001165</v>
       </c>
       <c r="H23">
-        <v>0.0768835518366827</v>
+        <v>2.548466659060828</v>
+      </c>
+      <c r="I23">
+        <v>5.568480786600949</v>
       </c>
       <c r="J23">
-        <v>0.04164295292991437</v>
+        <v>2.25767935113215</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>29.0836429540162</v>
-      </c>
-      <c r="C24">
-        <v>9.667613878962808</v>
+        <v>-0.0628458231774163</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>15.26693669571082</v>
+        <v>0.008764011651703414</v>
       </c>
       <c r="E24">
-        <v>19.11858586587187</v>
+        <v>0.008882694387101249</v>
       </c>
       <c r="F24">
-        <v>50.50199611141328</v>
+        <v>-0.02977285894526444</v>
       </c>
       <c r="G24">
-        <v>2.427942953003564</v>
+        <v>-0.00739094144241649</v>
       </c>
       <c r="H24">
-        <v>2.468485337580928</v>
+        <v>-0.006915052832246443</v>
+      </c>
+      <c r="I24">
+        <v>-0.04680704617218703</v>
       </c>
       <c r="J24">
-        <v>2.141316964223678</v>
+        <v>0.008043395692369093</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>-0.06099600086322601</v>
-      </c>
-      <c r="C25" t="s">
+        <v>-0.1308588593060638</v>
+      </c>
+      <c r="C25">
+        <v>-0.008764011651703414</v>
+      </c>
+      <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="D25">
-        <v>0.008458206609016979</v>
-      </c>
       <c r="E25">
-        <v>0.008573163487342194</v>
+        <v>0.008993226795665525</v>
       </c>
       <c r="F25">
-        <v>-0.02872640021723904</v>
+        <v>-0.05880705075024658</v>
       </c>
       <c r="G25">
-        <v>-0.007131026662455351</v>
+        <v>-0.007539716046119494</v>
       </c>
       <c r="H25">
-        <v>-0.006671938631790686</v>
+        <v>-0.007152463582014513</v>
+      </c>
+      <c r="I25">
+        <v>-0.0452702733819963</v>
       </c>
       <c r="J25">
-        <v>0.007764426056820343</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26">
-        <v>-0.1269250091575139</v>
-      </c>
-      <c r="C26">
-        <v>-0.008458206609016979</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26">
-        <v>0.008680040058490728</v>
-      </c>
-      <c r="F26">
-        <v>-0.05674091975591911</v>
-      </c>
-      <c r="G26">
-        <v>-0.00727483024953493</v>
-      </c>
-      <c r="H26">
-        <v>-0.006901249446038402</v>
-      </c>
-      <c r="J26">
-        <v>0.006717115544652307</v>
+        <v>0.006958211100291562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>